<commit_message>
lots of changes at 4:49am in the morning LMFAO
</commit_message>
<xml_diff>
--- a/personData.xlsx
+++ b/personData.xlsx
@@ -459,22 +459,10 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Niya</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Shroff</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
-        <v>500</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>